<commit_message>
atualização do dicionario de dados
</commit_message>
<xml_diff>
--- a/banco/documentacao/Dicionário de dados.xlsx
+++ b/banco/documentacao/Dicionário de dados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncunha\Documents\NetBeansProjects\PetAgenda\banco\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c.nunes\Desktop\pet\banco\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AA2C33-CD25-4C3F-BAF9-D5EAF51D088B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C234115-8F40-4910-A9C4-4FEF491913F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="196">
   <si>
     <t>cliente</t>
   </si>
@@ -286,9 +286,6 @@
     <t>Identifica a permissão que este usuário terá caso possua um perfil de acesso. Chave estrangeira da tabela "permissao".</t>
   </si>
   <si>
-    <t>id_local_atuacao</t>
-  </si>
-  <si>
     <t>Local de atuação do funcionário.</t>
   </si>
   <si>
@@ -602,13 +599,22 @@
   </si>
   <si>
     <t>Nome descritivo do serviço.</t>
+  </si>
+  <si>
+    <t>codigo_recup</t>
+  </si>
+  <si>
+    <t>"1234"</t>
+  </si>
+  <si>
+    <t>Codigo para o usuario recuperar a senha em cado de perda.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -653,6 +659,14 @@
       <u/>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -780,7 +794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -812,11 +826,6 @@
     <xf numFmtId="21" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -826,6 +835,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -833,6 +847,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1060,10 +1075,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G119"/>
+  <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="115" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="115" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1080,15 +1095,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1137,25 +1152,25 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="15" t="s">
+      <c r="B4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="15" t="s">
+      <c r="E4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1205,7 +1220,7 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>18</v>
@@ -1220,100 +1235,100 @@
         <v>12</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="G7" s="5" t="s">
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="B8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="15" t="s">
+      <c r="G8" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="E9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="15" t="s">
+      <c r="D10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="E10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="15" t="s">
+      <c r="G10" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="G10" s="15" t="s">
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="B11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="15" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="15" t="s">
+      <c r="G11" s="12" t="s">
         <v>105</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1382,7 +1397,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="14" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="18"/>
@@ -1417,7 +1432,7 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>9</v>
@@ -1656,15 +1671,15 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="13"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="16"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
@@ -1712,7 +1727,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>17</v>
       </c>
@@ -1735,7 +1750,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>15</v>
       </c>
@@ -1758,7 +1773,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>23</v>
       </c>
@@ -1778,10 +1793,10 @@
         <v>26</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>28</v>
       </c>
@@ -1804,7 +1819,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>82</v>
       </c>
@@ -1825,7 +1840,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>84</v>
       </c>
@@ -1847,8 +1862,9 @@
       <c r="G38" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J38" s="20"/>
+    </row>
+    <row r="39" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>86</v>
       </c>
@@ -1871,42 +1887,42 @@
         <v>87</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>77</v>
+        <v>194</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="13"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="16"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>1</v>
       </c>
@@ -1929,9 +1945,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>9</v>
@@ -1949,10 +1965,10 @@
         <v>13</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>17</v>
       </c>
@@ -1972,10 +1988,10 @@
         <v>77</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>23</v>
       </c>
@@ -1995,10 +2011,10 @@
         <v>26</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>28</v>
       </c>
@@ -2018,12 +2034,12 @@
         <v>30</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>18</v>
@@ -2038,36 +2054,36 @@
         <v>12</v>
       </c>
       <c r="F48" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G48" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F49" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G49" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>18</v>
@@ -2082,21 +2098,21 @@
         <v>12</v>
       </c>
       <c r="F50" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G50" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>20</v>
@@ -2105,15 +2121,15 @@
         <v>12</v>
       </c>
       <c r="F51" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G51" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>9</v>
@@ -2131,20 +2147,20 @@
         <v>77</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="55" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="13"/>
+      <c r="A55" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="16"/>
     </row>
     <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
@@ -2171,7 +2187,7 @@
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>9</v>
@@ -2189,7 +2205,7 @@
         <v>13</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2212,12 +2228,12 @@
         <v>77</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>9</v>
@@ -2235,18 +2251,18 @@
         <v>13</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="C60" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>113</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>20</v>
@@ -2258,12 +2274,12 @@
         <v>13</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>18</v>
@@ -2276,23 +2292,23 @@
         <v>12</v>
       </c>
       <c r="F61" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G61" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="13"/>
+      <c r="A63" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="16"/>
     </row>
     <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
@@ -2319,7 +2335,7 @@
     </row>
     <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>9</v>
@@ -2337,15 +2353,15 @@
         <v>13</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>121</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>13</v>
@@ -2357,15 +2373,15 @@
         <v>12</v>
       </c>
       <c r="F66" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G66" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>66</v>
@@ -2377,39 +2393,39 @@
         <v>20</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>68</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B68" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>130</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>131</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>9</v>
@@ -2427,12 +2443,12 @@
         <v>13</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>9</v>
@@ -2450,20 +2466,20 @@
         <v>13</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B72" s="12"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="13"/>
+      <c r="A72" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B72" s="15"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="16"/>
     </row>
     <row r="73" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
@@ -2490,7 +2506,7 @@
     </row>
     <row r="74" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>9</v>
@@ -2508,15 +2524,15 @@
         <v>13</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>13</v>
@@ -2528,21 +2544,21 @@
         <v>12</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>20</v>
@@ -2551,15 +2567,15 @@
         <v>12</v>
       </c>
       <c r="F76" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G76" s="5" t="s">
         <v>141</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>9</v>
@@ -2575,33 +2591,33 @@
         <v>13</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F78" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="G78" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="G78" s="5" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>18</v>
@@ -2614,7 +2630,7 @@
         <v>12</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>36</v>
@@ -2622,7 +2638,7 @@
     </row>
     <row r="80" spans="1:7" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>18</v>
@@ -2635,7 +2651,7 @@
         <v>12</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>38</v>
@@ -2643,51 +2659,51 @@
     </row>
     <row r="81" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F81" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G81" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="G81" s="5" t="s">
-        <v>155</v>
-      </c>
     </row>
     <row r="82" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="14" t="s">
+      <c r="A82" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B82" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="B82" s="15" t="s">
+      <c r="C82" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="C82" s="15" t="s">
+      <c r="D82" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E82" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F82" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G82" s="12" t="s">
         <v>176</v>
-      </c>
-      <c r="D82" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E82" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F82" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G82" s="15" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>9</v>
@@ -2705,12 +2721,12 @@
         <v>13</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>9</v>
@@ -2728,12 +2744,12 @@
         <v>13</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>9</v>
@@ -2751,20 +2767,20 @@
         <v>13</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="88" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="B88" s="12"/>
-      <c r="C88" s="12"/>
-      <c r="D88" s="12"/>
-      <c r="E88" s="12"/>
-      <c r="F88" s="12"/>
-      <c r="G88" s="13"/>
+      <c r="A88" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B88" s="15"/>
+      <c r="C88" s="15"/>
+      <c r="D88" s="15"/>
+      <c r="E88" s="15"/>
+      <c r="F88" s="15"/>
+      <c r="G88" s="16"/>
     </row>
     <row r="89" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
@@ -2791,7 +2807,7 @@
     </row>
     <row r="90" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>9</v>
@@ -2809,12 +2825,12 @@
         <v>13</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>18</v>
@@ -2823,24 +2839,24 @@
         <v>19</v>
       </c>
       <c r="D91" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="E91" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F91" s="5" t="s">
+      <c r="G91" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="G91" s="5" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B92" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>164</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>13</v>
@@ -2855,33 +2871,33 @@
         <v>0.7911111111111111</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C93" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>167</v>
       </c>
       <c r="D93" s="8"/>
       <c r="E93" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F93" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="G93" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="G93" s="5" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>9</v>
@@ -2890,7 +2906,7 @@
         <v>10</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E94" s="5" t="s">
         <v>12</v>
@@ -2899,20 +2915,20 @@
         <v>13</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="96" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="B96" s="12"/>
-      <c r="C96" s="12"/>
-      <c r="D96" s="12"/>
-      <c r="E96" s="12"/>
-      <c r="F96" s="12"/>
-      <c r="G96" s="13"/>
+      <c r="A96" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B96" s="15"/>
+      <c r="C96" s="15"/>
+      <c r="D96" s="15"/>
+      <c r="E96" s="15"/>
+      <c r="F96" s="15"/>
+      <c r="G96" s="16"/>
     </row>
     <row r="97" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
@@ -2939,7 +2955,7 @@
     </row>
     <row r="98" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>9</v>
@@ -2948,7 +2964,7 @@
         <v>10</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E98" s="5" t="s">
         <v>12</v>
@@ -2957,15 +2973,15 @@
         <v>13</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>13</v>
@@ -2980,12 +2996,12 @@
         <v>0.7911111111111111</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>9</v>
@@ -2994,7 +3010,7 @@
         <v>10</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E100" s="5" t="s">
         <v>12</v>
@@ -3003,7 +3019,7 @@
         <v>13</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3068,6 +3084,10 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A42:G42"/>
     <mergeCell ref="A88:G88"/>
     <mergeCell ref="A96:G96"/>
     <mergeCell ref="A104:G104"/>
@@ -3075,10 +3095,6 @@
     <mergeCell ref="A55:G55"/>
     <mergeCell ref="A63:G63"/>
     <mergeCell ref="A72:G72"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A42:G42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>